<commit_message>
REWIRING SCHEMATIC OVER HEAT CONCERN - picked and wired buck-converter - started FMEA analysis
</commit_message>
<xml_diff>
--- a/testing/BAJA_Electronics_FMEA.xlsx
+++ b/testing/BAJA_Electronics_FMEA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parry\Documents\GitHub\BCIT-BAJA\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parry\OneDrive\Documents\GitHub\BCIT-BAJA\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207767A7-F750-412B-8A88-397CB5476D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508A5885-7018-4842-A15D-08DD481DF3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="30912" windowHeight="16752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Item</t>
   </si>
@@ -43,82 +43,123 @@
     <t>Current Controls</t>
   </si>
   <si>
-    <t>5V Regulator</t>
-  </si>
-  <si>
     <t>Strain Gauge Wiring</t>
   </si>
   <si>
-    <t>Battery Fuse</t>
-  </si>
-  <si>
-    <t>Provide stable 5V for MCU &amp; sensors</t>
-  </si>
-  <si>
     <t>Transmit strain signal</t>
   </si>
   <si>
-    <t>Protect wiring</t>
-  </si>
-  <si>
     <t>Overheating / thermal shutdown</t>
   </si>
   <si>
     <t>Open circuit or noise pickup</t>
   </si>
   <si>
-    <t>Fuse blown due to short</t>
-  </si>
-  <si>
-    <t>MCU loses power, no data logging</t>
-  </si>
-  <si>
     <t>Incorrect strain readings</t>
   </si>
   <si>
-    <t>Entire system shut down</t>
-  </si>
-  <si>
-    <t>Undersized regulator or poor heat dissipation</t>
-  </si>
-  <si>
     <t>Connector failure, EMI, vibration</t>
   </si>
   <si>
-    <t>Short circuit downstream</t>
-  </si>
-  <si>
-    <t>Thermal pad, heatsink, current limit</t>
-  </si>
-  <si>
-    <t>Shielded twisted pair wiring, strain relief</t>
-  </si>
-  <si>
-    <t>Proper wire sizing, fuse rating</t>
-  </si>
-  <si>
-    <t>NUCLEO BOARD</t>
-  </si>
-  <si>
-    <t>Unable to receive power</t>
-  </si>
-  <si>
-    <t>Unable to receive power
-Sensor connections can become loose. 
-Peripherals connections can become loose</t>
-  </si>
-  <si>
-    <t>Controls all peripherals / regulates power</t>
-  </si>
-  <si>
-    <t>MCU won't boot, no system operation</t>
+    <t>Occurrence</t>
+  </si>
+  <si>
+    <t>Detection</t>
+  </si>
+  <si>
+    <t>RPN</t>
+  </si>
+  <si>
+    <t>Recommended Action</t>
+  </si>
+  <si>
+    <t>5V Voltage Regulator</t>
+  </si>
+  <si>
+    <t>other components get overly heated</t>
+  </si>
+  <si>
+    <t>Components break due to excessive heat</t>
+  </si>
+  <si>
+    <t>inefficient use of power</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>STM32 nucleo has built-in temperature sensor
+Or we can use a buck-convertor to not lose heat.</t>
+  </si>
+  <si>
+    <t>amplifier board</t>
+  </si>
+  <si>
+    <t>Amplifier board</t>
+  </si>
+  <si>
+    <t>Amplifies small signal of strain</t>
+  </si>
+  <si>
+    <t>reduces effect of noise onto wires, provides
+stability</t>
+  </si>
+  <si>
+    <t>unstable mounting</t>
+  </si>
+  <si>
+    <t>Capacitors, and RC filters.</t>
+  </si>
+  <si>
+    <t>Talk with johnny to see how mechanicals 
+manages this issue</t>
+  </si>
+  <si>
+    <t>Buck convertor</t>
+  </si>
+  <si>
+    <t>Steps voltage down to 5.5V for energy efficiency, 
+and to manage heat dissipation</t>
+  </si>
+  <si>
+    <t>Significant EMI can be generated</t>
+  </si>
+  <si>
+    <t>Cross talk between Analog traces</t>
+  </si>
+  <si>
+    <t>poorly routed traces</t>
+  </si>
+  <si>
+    <t>Lots of capacitors, amplifier board</t>
+  </si>
+  <si>
+    <t>wired incorrectly or soldered incorrectly</t>
+  </si>
+  <si>
+    <t>Does not properly regulate voltage</t>
+  </si>
+  <si>
+    <t>design mistake, poor soldering</t>
+  </si>
+  <si>
+    <t>0 ohm resistor to bypass buck, test point</t>
+  </si>
+  <si>
+    <t>less accurate readings</t>
+  </si>
+  <si>
+    <t>No voltage goes through to output</t>
+  </si>
+  <si>
+    <t>read datasheet in more detail to determine more options</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,23 +168,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -151,34 +209,43 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -485,156 +552,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.42578125" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.41796875" customWidth="1"/>
+    <col min="7" max="7" width="38.15625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" ht="135.30000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="4">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="6">
+        <v>10</v>
+      </c>
+      <c r="J2" s="6">
+        <v>800</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2">
+      <c r="D4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="9">
+        <v>7</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="9">
+        <v>3</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="9">
+        <v>6</v>
+      </c>
+      <c r="J4" s="9">
+        <v>168</v>
+      </c>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="9">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
+      <c r="F5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="9">
+        <v>9</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="10">
+        <v>5</v>
+      </c>
+      <c r="J5" s="10">
+        <v>360</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="10">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="10">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="10">
+        <v>4</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="10">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
+      <c r="J7" s="10">
+        <v>84</v>
+      </c>
+      <c r="K7" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
+    <row r="8" spans="1:11" ht="87" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="10">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="10">
+        <v>7</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="10">
+        <v>2</v>
+      </c>
+      <c r="J8" s="10">
+        <v>140</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>